<commit_message>
Changes on Modal Contacts format number
</commit_message>
<xml_diff>
--- a/frontend/public/import-contatos.xlsx
+++ b/frontend/public/import-contatos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -31,13 +31,7 @@
     <t xml:space="preserve">Contato 1</t>
   </si>
   <si>
-    <t xml:space="preserve">(31) 99999-9999</t>
-  </si>
-  <si>
     <t xml:space="preserve">Contato 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(41) 99999-9999</t>
   </si>
 </sst>
 </file>
@@ -52,6 +46,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,12 +131,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
   </cols>
   <sheetData>
@@ -157,16 +152,16 @@
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
+      <c r="B2" s="0" t="n">
+        <v>553199999999</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
+      <c r="B3" s="0" t="n">
+        <v>554199999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>